<commit_message>
slack text length count
</commit_message>
<xml_diff>
--- a/data/계량기_점검_교체_리스트_통합.xlsx
+++ b/data/계량기_점검_교체_리스트_통합.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jis\Desktop\민수계기_모니터링_리스트\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7A8827-D244-40F4-A308-9CA8027FB5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05627EE7-0A4E-4FD4-9CF4-016DE9AA738D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D0F43CBF-36CC-4187-9068-1B8FD29C3464}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D0F43CBF-36CC-4187-9068-1B8FD29C3464}"/>
   </bookViews>
   <sheets>
     <sheet name="요청리스트" sheetId="1" r:id="rId1"/>
     <sheet name="점검리스트" sheetId="2" r:id="rId2"/>
+    <sheet name="정상확인리스트" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">점검리스트!$A$1:$M$183</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2063" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2279" uniqueCount="837">
   <si>
     <t>LG 엘지빌리지2차 (경기도 용인시 수지구 수지로113번길 15)</t>
   </si>
@@ -2732,6 +2733,326 @@
   <si>
     <t>미터 ID</t>
   </si>
+  <si>
+    <t>A0537130282</t>
+  </si>
+  <si>
+    <t>A0537132659</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0537132663</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0537137908</t>
+  </si>
+  <si>
+    <t>관리사무소에 차단기 교체 요청</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>101동</t>
+  </si>
+  <si>
+    <t>1201호</t>
+  </si>
+  <si>
+    <t>1202호</t>
+  </si>
+  <si>
+    <t>A0537120349</t>
+  </si>
+  <si>
+    <t>1304호</t>
+  </si>
+  <si>
+    <t>A0537121735</t>
+  </si>
+  <si>
+    <t>1502호</t>
+  </si>
+  <si>
+    <t>102동</t>
+  </si>
+  <si>
+    <t>401호</t>
+  </si>
+  <si>
+    <t>A0537140416</t>
+  </si>
+  <si>
+    <t>603호</t>
+  </si>
+  <si>
+    <t>A0537131502</t>
+  </si>
+  <si>
+    <t>605호</t>
+  </si>
+  <si>
+    <t>A0537124080</t>
+  </si>
+  <si>
+    <t>103동</t>
+  </si>
+  <si>
+    <t>202호</t>
+  </si>
+  <si>
+    <t>A0537139499</t>
+  </si>
+  <si>
+    <t>104동</t>
+  </si>
+  <si>
+    <t>1005호</t>
+  </si>
+  <si>
+    <t>A0537144471</t>
+  </si>
+  <si>
+    <t>1105호</t>
+  </si>
+  <si>
+    <t>A0537144476</t>
+  </si>
+  <si>
+    <t>1106호</t>
+  </si>
+  <si>
+    <t>A0537072621</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0537072787</t>
+  </si>
+  <si>
+    <t>A0537072879</t>
+  </si>
+  <si>
+    <t>A0537072741</t>
+  </si>
+  <si>
+    <t>A0537088281</t>
+  </si>
+  <si>
+    <t>A0537036187</t>
+  </si>
+  <si>
+    <t>A0537070303</t>
+  </si>
+  <si>
+    <t>A0537087916</t>
+  </si>
+  <si>
+    <t>A0537070641</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0537036193</t>
+  </si>
+  <si>
+    <t>A0537068551</t>
+  </si>
+  <si>
+    <t>A0537087840</t>
+  </si>
+  <si>
+    <t>A0537008590</t>
+  </si>
+  <si>
+    <t>A0537077243</t>
+  </si>
+  <si>
+    <t>A0537041735</t>
+  </si>
+  <si>
+    <t>A0537091549</t>
+  </si>
+  <si>
+    <t>A0537151133</t>
+  </si>
+  <si>
+    <t>A0537073899</t>
+  </si>
+  <si>
+    <t>A0537049888</t>
+  </si>
+  <si>
+    <t>A0537046154</t>
+  </si>
+  <si>
+    <t>A0537044208</t>
+  </si>
+  <si>
+    <t>A0537043265</t>
+  </si>
+  <si>
+    <t>A0537155358</t>
+  </si>
+  <si>
+    <t>A0537044715</t>
+  </si>
+  <si>
+    <t>A0537153752</t>
+  </si>
+  <si>
+    <t>A0537097670</t>
+  </si>
+  <si>
+    <t>A0537087980</t>
+  </si>
+  <si>
+    <t>A0537078852</t>
+  </si>
+  <si>
+    <t>A0537094251</t>
+  </si>
+  <si>
+    <t>A0537095406</t>
+  </si>
+  <si>
+    <t>A0537097802</t>
+  </si>
+  <si>
+    <t>A0537087558</t>
+  </si>
+  <si>
+    <t>A0537036381</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  기산/계산한미삼오E</t>
+  </si>
+  <si>
+    <t>A0537111723</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  도봉동아에코빌</t>
+  </si>
+  <si>
+    <t>A0537067735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  봉담한신</t>
+  </si>
+  <si>
+    <t>A0537018368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  산곡5차현대</t>
+  </si>
+  <si>
+    <t>A0537154223</t>
+  </si>
+  <si>
+    <t>A0537160646</t>
+  </si>
+  <si>
+    <t>A0537160654</t>
+  </si>
+  <si>
+    <t>A0537160809</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  상계주공7단지</t>
+  </si>
+  <si>
+    <t>A0537007788</t>
+  </si>
+  <si>
+    <t>A0537043393</t>
+  </si>
+  <si>
+    <t>A0537034827</t>
+  </si>
+  <si>
+    <t>A0537032504</t>
+  </si>
+  <si>
+    <t>A0537041142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  석사2지구</t>
+  </si>
+  <si>
+    <t>A0537074034</t>
+  </si>
+  <si>
+    <t>A0537026766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  석수경남아너스빌</t>
+  </si>
+  <si>
+    <t>A0537126760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  쌍용예가</t>
+  </si>
+  <si>
+    <t>A0537123105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  옥련한국</t>
+  </si>
+  <si>
+    <t>A0537117128</t>
+  </si>
+  <si>
+    <t>A0537118657</t>
+  </si>
+  <si>
+    <t>A0537074348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  우만주공4단지</t>
+  </si>
+  <si>
+    <t>A0537136712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  중앙주공9단지</t>
+  </si>
+  <si>
+    <t>A0537008984</t>
+  </si>
+  <si>
+    <t>A0537008289</t>
+  </si>
+  <si>
+    <t>A0537008282</t>
+  </si>
+  <si>
+    <t>A0537008640</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  진건금강</t>
+  </si>
+  <si>
+    <t>A0537146569</t>
+  </si>
+  <si>
+    <t>A0537094207</t>
+  </si>
+  <si>
+    <t>문래건영 (서울시 영등포구 문래로 94-7)</t>
+  </si>
+  <si>
+    <t>상계주공3단지 (서울특별시 노원구 동일로 1389)</t>
+  </si>
+  <si>
+    <t>신월대림 (서울특별시 양천구 오목로13길 7)</t>
+  </si>
+  <si>
+    <t>자양경남아너스빌 (서울특별시 광진구 자양로3길 55)</t>
+  </si>
+  <si>
+    <t>공도부영 (경기도 안성시 만수로 31)</t>
+  </si>
+  <si>
+    <t>A0537089514</t>
+  </si>
 </sst>
 </file>
 
@@ -2740,7 +3061,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2855,8 +3176,24 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2869,8 +3206,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -3116,19 +3471,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="dashed">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="dashed">
         <color indexed="64"/>
       </left>
@@ -3150,7 +3492,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3331,13 +3673,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3388,6 +3727,51 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3409,12 +3793,75 @@
     <xf numFmtId="176" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="74">
+  <dxfs count="80">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4465,10 +4912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A31A018-25B8-4F7A-88E3-890EB1272FDE}">
-  <dimension ref="A1:L487"/>
+  <dimension ref="A1:L518"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D2"/>
+    <sheetView topLeftCell="A488" workbookViewId="0">
+      <selection activeCell="H499" sqref="H499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4484,38 +4931,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="95" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="95" t="s">
         <v>210</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="95" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="95" t="s">
         <v>212</v>
       </c>
       <c r="E1" s="16"/>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="95" t="s">
         <v>213</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="95" t="s">
         <v>214</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="H1" s="95" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickBot="1">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
       <c r="E2" s="17"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="8" t="s">
@@ -8377,7 +8824,7 @@
       </c>
     </row>
     <row r="206" spans="1:6">
-      <c r="A206" s="73" t="s">
+      <c r="A206" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B206" s="19">
@@ -8386,16 +8833,16 @@
       <c r="C206" s="19">
         <v>1001</v>
       </c>
-      <c r="D206" s="74" t="s">
+      <c r="D206" s="73" t="s">
         <v>216</v>
       </c>
-      <c r="E206" s="74"/>
+      <c r="E206" s="73"/>
       <c r="F206" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="207" spans="1:6">
-      <c r="A207" s="73" t="s">
+      <c r="A207" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B207" s="19">
@@ -8404,16 +8851,16 @@
       <c r="C207" s="19">
         <v>901</v>
       </c>
-      <c r="D207" s="74" t="s">
+      <c r="D207" s="73" t="s">
         <v>217</v>
       </c>
-      <c r="E207" s="74"/>
+      <c r="E207" s="73"/>
       <c r="F207" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="208" spans="1:6">
-      <c r="A208" s="73" t="s">
+      <c r="A208" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B208" s="19">
@@ -8422,16 +8869,16 @@
       <c r="C208" s="19">
         <v>401</v>
       </c>
-      <c r="D208" s="74" t="s">
+      <c r="D208" s="73" t="s">
         <v>218</v>
       </c>
-      <c r="E208" s="74"/>
+      <c r="E208" s="73"/>
       <c r="F208" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="209" spans="1:6">
-      <c r="A209" s="73" t="s">
+      <c r="A209" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B209" s="19">
@@ -8440,16 +8887,16 @@
       <c r="C209" s="19">
         <v>201</v>
       </c>
-      <c r="D209" s="74" t="s">
+      <c r="D209" s="73" t="s">
         <v>219</v>
       </c>
-      <c r="E209" s="74"/>
+      <c r="E209" s="73"/>
       <c r="F209" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="210" spans="1:6">
-      <c r="A210" s="73" t="s">
+      <c r="A210" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B210" s="19">
@@ -8458,16 +8905,16 @@
       <c r="C210" s="19">
         <v>1001</v>
       </c>
-      <c r="D210" s="74" t="s">
+      <c r="D210" s="73" t="s">
         <v>220</v>
       </c>
-      <c r="E210" s="74"/>
+      <c r="E210" s="73"/>
       <c r="F210" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="211" spans="1:6">
-      <c r="A211" s="73" t="s">
+      <c r="A211" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B211" s="19">
@@ -8476,16 +8923,16 @@
       <c r="C211" s="19">
         <v>501</v>
       </c>
-      <c r="D211" s="74" t="s">
+      <c r="D211" s="73" t="s">
         <v>221</v>
       </c>
-      <c r="E211" s="74"/>
+      <c r="E211" s="73"/>
       <c r="F211" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="212" spans="1:6">
-      <c r="A212" s="73" t="s">
+      <c r="A212" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B212" s="19">
@@ -8494,16 +8941,16 @@
       <c r="C212" s="19">
         <v>901</v>
       </c>
-      <c r="D212" s="74" t="s">
+      <c r="D212" s="73" t="s">
         <v>222</v>
       </c>
-      <c r="E212" s="74"/>
+      <c r="E212" s="73"/>
       <c r="F212" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="213" spans="1:6">
-      <c r="A213" s="73" t="s">
+      <c r="A213" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B213" s="19">
@@ -8512,16 +8959,16 @@
       <c r="C213" s="19">
         <v>801</v>
       </c>
-      <c r="D213" s="74" t="s">
+      <c r="D213" s="73" t="s">
         <v>223</v>
       </c>
-      <c r="E213" s="74"/>
+      <c r="E213" s="73"/>
       <c r="F213" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="214" spans="1:6">
-      <c r="A214" s="73" t="s">
+      <c r="A214" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B214" s="19">
@@ -8530,16 +8977,16 @@
       <c r="C214" s="19">
         <v>1001</v>
       </c>
-      <c r="D214" s="74" t="s">
+      <c r="D214" s="73" t="s">
         <v>224</v>
       </c>
-      <c r="E214" s="74"/>
+      <c r="E214" s="73"/>
       <c r="F214" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="215" spans="1:6">
-      <c r="A215" s="73" t="s">
+      <c r="A215" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B215" s="19">
@@ -8548,16 +8995,16 @@
       <c r="C215" s="19">
         <v>601</v>
       </c>
-      <c r="D215" s="74" t="s">
+      <c r="D215" s="73" t="s">
         <v>225</v>
       </c>
-      <c r="E215" s="74"/>
+      <c r="E215" s="73"/>
       <c r="F215" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="216" spans="1:6">
-      <c r="A216" s="73" t="s">
+      <c r="A216" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B216" s="19">
@@ -8566,16 +9013,16 @@
       <c r="C216" s="19">
         <v>901</v>
       </c>
-      <c r="D216" s="74" t="s">
+      <c r="D216" s="73" t="s">
         <v>226</v>
       </c>
-      <c r="E216" s="74"/>
+      <c r="E216" s="73"/>
       <c r="F216" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="217" spans="1:6">
-      <c r="A217" s="73" t="s">
+      <c r="A217" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B217" s="19">
@@ -8584,16 +9031,16 @@
       <c r="C217" s="19">
         <v>901</v>
       </c>
-      <c r="D217" s="74" t="s">
+      <c r="D217" s="73" t="s">
         <v>227</v>
       </c>
-      <c r="E217" s="74"/>
+      <c r="E217" s="73"/>
       <c r="F217" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="218" spans="1:6">
-      <c r="A218" s="73" t="s">
+      <c r="A218" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B218" s="19">
@@ -8602,16 +9049,16 @@
       <c r="C218" s="19">
         <v>201</v>
       </c>
-      <c r="D218" s="74" t="s">
+      <c r="D218" s="73" t="s">
         <v>228</v>
       </c>
-      <c r="E218" s="74"/>
+      <c r="E218" s="73"/>
       <c r="F218" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="219" spans="1:6">
-      <c r="A219" s="73" t="s">
+      <c r="A219" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B219" s="19">
@@ -8620,16 +9067,16 @@
       <c r="C219" s="19">
         <v>201</v>
       </c>
-      <c r="D219" s="74" t="s">
+      <c r="D219" s="73" t="s">
         <v>229</v>
       </c>
-      <c r="E219" s="74"/>
+      <c r="E219" s="73"/>
       <c r="F219" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="220" spans="1:6">
-      <c r="A220" s="73" t="s">
+      <c r="A220" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B220" s="19">
@@ -8638,16 +9085,16 @@
       <c r="C220" s="19">
         <v>301</v>
       </c>
-      <c r="D220" s="74" t="s">
+      <c r="D220" s="73" t="s">
         <v>230</v>
       </c>
-      <c r="E220" s="74"/>
+      <c r="E220" s="73"/>
       <c r="F220" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="221" spans="1:6">
-      <c r="A221" s="73" t="s">
+      <c r="A221" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B221" s="19">
@@ -8665,7 +9112,7 @@
       </c>
     </row>
     <row r="222" spans="1:6">
-      <c r="A222" s="73" t="s">
+      <c r="A222" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B222" s="19">
@@ -8683,7 +9130,7 @@
       </c>
     </row>
     <row r="223" spans="1:6">
-      <c r="A223" s="73" t="s">
+      <c r="A223" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B223" s="19">
@@ -8701,7 +9148,7 @@
       </c>
     </row>
     <row r="224" spans="1:6">
-      <c r="A224" s="73" t="s">
+      <c r="A224" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B224" s="19">
@@ -8710,16 +9157,16 @@
       <c r="C224" s="19">
         <v>1001</v>
       </c>
-      <c r="D224" s="74" t="s">
+      <c r="D224" s="73" t="s">
         <v>234</v>
       </c>
-      <c r="E224" s="74"/>
+      <c r="E224" s="73"/>
       <c r="F224" s="18">
         <v>45146</v>
       </c>
     </row>
     <row r="225" spans="1:12">
-      <c r="A225" s="73" t="s">
+      <c r="A225" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B225" s="19">
@@ -8735,7 +9182,7 @@
         <v>45146</v>
       </c>
       <c r="G225" s="13"/>
-      <c r="H225" s="63" t="s">
+      <c r="H225" s="62" t="s">
         <v>238</v>
       </c>
       <c r="I225" s="59"/>
@@ -8744,7 +9191,7 @@
       <c r="L225" s="59"/>
     </row>
     <row r="226" spans="1:12">
-      <c r="A226" s="73" t="s">
+      <c r="A226" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B226" s="19">
@@ -8760,7 +9207,7 @@
         <v>45146</v>
       </c>
       <c r="G226" s="13"/>
-      <c r="H226" s="63" t="s">
+      <c r="H226" s="62" t="s">
         <v>239</v>
       </c>
       <c r="I226" s="59"/>
@@ -8769,7 +9216,7 @@
       <c r="L226" s="59"/>
     </row>
     <row r="227" spans="1:12">
-      <c r="A227" s="73" t="s">
+      <c r="A227" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B227" s="19">
@@ -8785,7 +9232,7 @@
         <v>45146</v>
       </c>
       <c r="G227" s="13"/>
-      <c r="H227" s="63" t="s">
+      <c r="H227" s="62" t="s">
         <v>240</v>
       </c>
       <c r="I227" s="59"/>
@@ -8794,7 +9241,7 @@
       <c r="L227" s="59"/>
     </row>
     <row r="228" spans="1:12">
-      <c r="A228" s="73" t="s">
+      <c r="A228" s="72" t="s">
         <v>73</v>
       </c>
       <c r="B228" s="19">
@@ -8810,7 +9257,7 @@
         <v>45146</v>
       </c>
       <c r="G228" s="13"/>
-      <c r="H228" s="63" t="s">
+      <c r="H228" s="62" t="s">
         <v>241</v>
       </c>
       <c r="I228" s="59"/>
@@ -8835,7 +9282,7 @@
         <v>45146</v>
       </c>
       <c r="G229" s="13"/>
-      <c r="H229" s="63" t="s">
+      <c r="H229" s="62" t="s">
         <v>239</v>
       </c>
       <c r="I229" s="59"/>
@@ -8844,7 +9291,7 @@
       <c r="L229" s="59"/>
     </row>
     <row r="230" spans="1:12">
-      <c r="A230" s="64" t="s">
+      <c r="A230" s="63" t="s">
         <v>245</v>
       </c>
       <c r="B230" s="19">
@@ -8860,7 +9307,7 @@
         <v>45146</v>
       </c>
       <c r="G230" s="13"/>
-      <c r="H230" s="63" t="s">
+      <c r="H230" s="62" t="s">
         <v>552</v>
       </c>
       <c r="I230" s="59"/>
@@ -8869,7 +9316,7 @@
       <c r="L230" s="59"/>
     </row>
     <row r="231" spans="1:12">
-      <c r="A231" s="64" t="s">
+      <c r="A231" s="63" t="s">
         <v>244</v>
       </c>
       <c r="B231" s="19">
@@ -8885,7 +9332,7 @@
         <v>45146</v>
       </c>
       <c r="G231" s="13"/>
-      <c r="H231" s="63" t="s">
+      <c r="H231" s="62" t="s">
         <v>236</v>
       </c>
       <c r="I231" s="59"/>
@@ -9568,7 +10015,7 @@
       </c>
     </row>
     <row r="266" spans="1:8">
-      <c r="A266" s="80" t="s">
+      <c r="A266" s="94" t="s">
         <v>35</v>
       </c>
       <c r="B266" s="13">
@@ -9588,7 +10035,7 @@
       </c>
     </row>
     <row r="267" spans="1:8">
-      <c r="A267" s="80"/>
+      <c r="A267" s="94"/>
       <c r="B267" s="13">
         <v>101</v>
       </c>
@@ -9606,7 +10053,7 @@
       </c>
     </row>
     <row r="268" spans="1:8">
-      <c r="A268" s="80"/>
+      <c r="A268" s="94"/>
       <c r="B268" s="13">
         <v>101</v>
       </c>
@@ -9624,7 +10071,7 @@
       </c>
     </row>
     <row r="269" spans="1:8">
-      <c r="A269" s="80"/>
+      <c r="A269" s="94"/>
       <c r="B269" s="13">
         <v>101</v>
       </c>
@@ -9642,7 +10089,7 @@
       </c>
     </row>
     <row r="270" spans="1:8">
-      <c r="A270" s="80"/>
+      <c r="A270" s="94"/>
       <c r="B270" s="13">
         <v>101</v>
       </c>
@@ -9660,7 +10107,7 @@
       </c>
     </row>
     <row r="271" spans="1:8">
-      <c r="A271" s="80"/>
+      <c r="A271" s="94"/>
       <c r="B271" s="13">
         <v>125</v>
       </c>
@@ -9676,7 +10123,7 @@
       </c>
     </row>
     <row r="272" spans="1:8">
-      <c r="A272" s="80"/>
+      <c r="A272" s="94"/>
       <c r="B272" s="13">
         <v>102</v>
       </c>
@@ -9694,7 +10141,7 @@
       </c>
     </row>
     <row r="273" spans="1:8">
-      <c r="A273" s="80"/>
+      <c r="A273" s="94"/>
       <c r="B273" s="13">
         <v>123</v>
       </c>
@@ -9712,7 +10159,7 @@
       </c>
     </row>
     <row r="274" spans="1:8">
-      <c r="A274" s="80"/>
+      <c r="A274" s="94"/>
       <c r="B274" s="13">
         <v>115</v>
       </c>
@@ -9730,7 +10177,7 @@
       </c>
     </row>
     <row r="275" spans="1:8">
-      <c r="A275" s="80"/>
+      <c r="A275" s="94"/>
       <c r="B275" s="13">
         <v>105</v>
       </c>
@@ -9748,7 +10195,7 @@
       </c>
     </row>
     <row r="276" spans="1:8">
-      <c r="A276" s="80"/>
+      <c r="A276" s="94"/>
       <c r="B276" s="13">
         <v>106</v>
       </c>
@@ -9766,7 +10213,7 @@
       </c>
     </row>
     <row r="277" spans="1:8">
-      <c r="A277" s="80"/>
+      <c r="A277" s="94"/>
       <c r="B277" s="13">
         <v>106</v>
       </c>
@@ -9784,7 +10231,7 @@
       </c>
     </row>
     <row r="278" spans="1:8">
-      <c r="A278" s="80"/>
+      <c r="A278" s="94"/>
       <c r="B278" s="13">
         <v>111</v>
       </c>
@@ -9802,7 +10249,7 @@
       </c>
     </row>
     <row r="279" spans="1:8">
-      <c r="A279" s="80"/>
+      <c r="A279" s="94"/>
       <c r="B279" s="13">
         <v>116</v>
       </c>
@@ -9820,7 +10267,7 @@
       </c>
     </row>
     <row r="280" spans="1:8">
-      <c r="A280" s="80"/>
+      <c r="A280" s="94"/>
       <c r="B280" s="13">
         <v>102</v>
       </c>
@@ -12145,7 +12592,7 @@
       </c>
     </row>
     <row r="399" spans="1:8">
-      <c r="A399" s="75" t="s">
+      <c r="A399" s="74" t="s">
         <v>492</v>
       </c>
       <c r="B399" s="19">
@@ -12165,7 +12612,7 @@
       </c>
     </row>
     <row r="400" spans="1:8">
-      <c r="A400" s="75" t="s">
+      <c r="A400" s="74" t="s">
         <v>492</v>
       </c>
       <c r="B400" s="19">
@@ -12225,7 +12672,7 @@
       </c>
     </row>
     <row r="403" spans="1:8">
-      <c r="A403" s="65" t="s">
+      <c r="A403" s="64" t="s">
         <v>500</v>
       </c>
       <c r="B403" s="23">
@@ -12234,7 +12681,7 @@
       <c r="C403" s="23">
         <v>401</v>
       </c>
-      <c r="D403" s="76" t="s">
+      <c r="D403" s="75" t="s">
         <v>242</v>
       </c>
       <c r="F403" s="18">
@@ -12242,7 +12689,7 @@
       </c>
     </row>
     <row r="404" spans="1:8">
-      <c r="A404" s="65" t="s">
+      <c r="A404" s="64" t="s">
         <v>501</v>
       </c>
       <c r="B404" s="23">
@@ -12259,7 +12706,7 @@
       </c>
     </row>
     <row r="405" spans="1:8">
-      <c r="A405" s="65" t="s">
+      <c r="A405" s="64" t="s">
         <v>503</v>
       </c>
       <c r="B405" s="23">
@@ -12268,7 +12715,7 @@
       <c r="C405" s="23">
         <v>1101</v>
       </c>
-      <c r="D405" s="76" t="s">
+      <c r="D405" s="75" t="s">
         <v>504</v>
       </c>
       <c r="F405" s="18">
@@ -12276,7 +12723,7 @@
       </c>
     </row>
     <row r="406" spans="1:8">
-      <c r="A406" s="65" t="s">
+      <c r="A406" s="64" t="s">
         <v>505</v>
       </c>
       <c r="B406" s="23">
@@ -12293,7 +12740,7 @@
       </c>
     </row>
     <row r="407" spans="1:8">
-      <c r="A407" s="66" t="s">
+      <c r="A407" s="65" t="s">
         <v>273</v>
       </c>
       <c r="B407" s="24">
@@ -12310,7 +12757,7 @@
       </c>
     </row>
     <row r="408" spans="1:8">
-      <c r="A408" s="66" t="s">
+      <c r="A408" s="65" t="s">
         <v>273</v>
       </c>
       <c r="B408" s="24">
@@ -12327,7 +12774,7 @@
       </c>
     </row>
     <row r="409" spans="1:8">
-      <c r="A409" s="66" t="s">
+      <c r="A409" s="65" t="s">
         <v>508</v>
       </c>
       <c r="B409" s="23">
@@ -12344,7 +12791,7 @@
       </c>
     </row>
     <row r="410" spans="1:8">
-      <c r="A410" s="66" t="s">
+      <c r="A410" s="65" t="s">
         <v>508</v>
       </c>
       <c r="B410" s="25">
@@ -12361,7 +12808,7 @@
       </c>
     </row>
     <row r="411" spans="1:8">
-      <c r="A411" s="65" t="s">
+      <c r="A411" s="64" t="s">
         <v>59</v>
       </c>
       <c r="B411" s="24">
@@ -12381,7 +12828,7 @@
       </c>
     </row>
     <row r="412" spans="1:8">
-      <c r="A412" s="65" t="s">
+      <c r="A412" s="64" t="s">
         <v>59</v>
       </c>
       <c r="B412" s="25">
@@ -12401,7 +12848,7 @@
       </c>
     </row>
     <row r="413" spans="1:8">
-      <c r="A413" s="65" t="s">
+      <c r="A413" s="64" t="s">
         <v>512</v>
       </c>
       <c r="B413" s="25">
@@ -12418,7 +12865,7 @@
       </c>
     </row>
     <row r="414" spans="1:8">
-      <c r="A414" s="66" t="s">
+      <c r="A414" s="65" t="s">
         <v>22</v>
       </c>
       <c r="B414" s="23">
@@ -12438,7 +12885,7 @@
       </c>
     </row>
     <row r="415" spans="1:8">
-      <c r="A415" s="66" t="s">
+      <c r="A415" s="65" t="s">
         <v>22</v>
       </c>
       <c r="B415" s="23">
@@ -12458,7 +12905,7 @@
       </c>
     </row>
     <row r="416" spans="1:8">
-      <c r="A416" s="66" t="s">
+      <c r="A416" s="65" t="s">
         <v>22</v>
       </c>
       <c r="B416" s="23">
@@ -12478,7 +12925,7 @@
       </c>
     </row>
     <row r="417" spans="1:8">
-      <c r="A417" s="65" t="s">
+      <c r="A417" s="64" t="s">
         <v>517</v>
       </c>
       <c r="B417" s="25">
@@ -12498,7 +12945,7 @@
       </c>
     </row>
     <row r="418" spans="1:8">
-      <c r="A418" s="66" t="s">
+      <c r="A418" s="65" t="s">
         <v>519</v>
       </c>
       <c r="B418" s="23">
@@ -12515,7 +12962,7 @@
       </c>
     </row>
     <row r="419" spans="1:8">
-      <c r="A419" s="67" t="s">
+      <c r="A419" s="66" t="s">
         <v>521</v>
       </c>
       <c r="B419" s="13">
@@ -12532,7 +12979,7 @@
       </c>
     </row>
     <row r="420" spans="1:8">
-      <c r="A420" s="79" t="s">
+      <c r="A420" s="93" t="s">
         <v>522</v>
       </c>
       <c r="B420" s="13">
@@ -12549,7 +12996,7 @@
       </c>
     </row>
     <row r="421" spans="1:8">
-      <c r="A421" s="79"/>
+      <c r="A421" s="93"/>
       <c r="B421" s="13">
         <v>127</v>
       </c>
@@ -12564,7 +13011,7 @@
       </c>
     </row>
     <row r="422" spans="1:8">
-      <c r="A422" s="79"/>
+      <c r="A422" s="93"/>
       <c r="B422" s="13">
         <v>112</v>
       </c>
@@ -12579,7 +13026,7 @@
       </c>
     </row>
     <row r="423" spans="1:8">
-      <c r="A423" s="79"/>
+      <c r="A423" s="93"/>
       <c r="B423" s="13">
         <v>114</v>
       </c>
@@ -12594,7 +13041,7 @@
       </c>
     </row>
     <row r="424" spans="1:8">
-      <c r="A424" s="67" t="s">
+      <c r="A424" s="66" t="s">
         <v>523</v>
       </c>
       <c r="B424" s="13">
@@ -12611,7 +13058,7 @@
       </c>
     </row>
     <row r="425" spans="1:8">
-      <c r="A425" s="67" t="s">
+      <c r="A425" s="66" t="s">
         <v>524</v>
       </c>
       <c r="B425" s="13">
@@ -12662,7 +13109,7 @@
       </c>
     </row>
     <row r="428" spans="1:8">
-      <c r="A428" s="75" t="s">
+      <c r="A428" s="74" t="s">
         <v>255</v>
       </c>
       <c r="B428" s="19">
@@ -12682,7 +13129,7 @@
       </c>
     </row>
     <row r="429" spans="1:8">
-      <c r="A429" s="75" t="s">
+      <c r="A429" s="74" t="s">
         <v>255</v>
       </c>
       <c r="B429" s="19">
@@ -12702,7 +13149,7 @@
       </c>
     </row>
     <row r="430" spans="1:8">
-      <c r="A430" s="75" t="s">
+      <c r="A430" s="74" t="s">
         <v>531</v>
       </c>
       <c r="B430" s="19">
@@ -12711,7 +13158,7 @@
       <c r="C430" s="19">
         <v>803</v>
       </c>
-      <c r="D430" s="77" t="s">
+      <c r="D430" s="76" t="s">
         <v>532</v>
       </c>
       <c r="F430" s="18">
@@ -12722,7 +13169,7 @@
       </c>
     </row>
     <row r="431" spans="1:8">
-      <c r="A431" s="75" t="s">
+      <c r="A431" s="74" t="s">
         <v>256</v>
       </c>
       <c r="B431" s="19">
@@ -12731,7 +13178,7 @@
       <c r="C431" s="19">
         <v>1102</v>
       </c>
-      <c r="D431" s="77" t="s">
+      <c r="D431" s="76" t="s">
         <v>534</v>
       </c>
       <c r="F431" s="18">
@@ -12742,7 +13189,7 @@
       </c>
     </row>
     <row r="432" spans="1:8">
-      <c r="A432" s="75" t="s">
+      <c r="A432" s="74" t="s">
         <v>536</v>
       </c>
       <c r="B432" s="19">
@@ -12751,7 +13198,7 @@
       <c r="C432" s="19">
         <v>704</v>
       </c>
-      <c r="D432" s="77" t="s">
+      <c r="D432" s="76" t="s">
         <v>490</v>
       </c>
       <c r="F432" s="18">
@@ -12762,7 +13209,7 @@
       </c>
     </row>
     <row r="433" spans="1:8">
-      <c r="A433" s="75" t="s">
+      <c r="A433" s="74" t="s">
         <v>536</v>
       </c>
       <c r="B433" s="19">
@@ -12771,7 +13218,7 @@
       <c r="C433" s="19">
         <v>1206</v>
       </c>
-      <c r="D433" s="78" t="s">
+      <c r="D433" s="77" t="s">
         <v>539</v>
       </c>
       <c r="F433" s="18">
@@ -12782,7 +13229,7 @@
       </c>
     </row>
     <row r="434" spans="1:8">
-      <c r="A434" s="75" t="s">
+      <c r="A434" s="74" t="s">
         <v>536</v>
       </c>
       <c r="B434" s="19">
@@ -12791,7 +13238,7 @@
       <c r="C434" s="19">
         <v>304</v>
       </c>
-      <c r="D434" s="78" t="s">
+      <c r="D434" s="77" t="s">
         <v>540</v>
       </c>
       <c r="F434" s="18">
@@ -13090,7 +13537,7 @@
       </c>
     </row>
     <row r="450" spans="1:6">
-      <c r="A450" s="68" t="s">
+      <c r="A450" s="67" t="s">
         <v>86</v>
       </c>
       <c r="B450" s="27">
@@ -13107,7 +13554,7 @@
       </c>
     </row>
     <row r="451" spans="1:6">
-      <c r="A451" s="68" t="s">
+      <c r="A451" s="67" t="s">
         <v>572</v>
       </c>
       <c r="B451" s="27">
@@ -13124,7 +13571,7 @@
       </c>
     </row>
     <row r="452" spans="1:6">
-      <c r="A452" s="69" t="s">
+      <c r="A452" s="68" t="s">
         <v>22</v>
       </c>
       <c r="B452" s="23">
@@ -13141,7 +13588,7 @@
       </c>
     </row>
     <row r="453" spans="1:6">
-      <c r="A453" s="69" t="s">
+      <c r="A453" s="68" t="s">
         <v>700</v>
       </c>
       <c r="B453" s="24">
@@ -13158,7 +13605,7 @@
       </c>
     </row>
     <row r="454" spans="1:6">
-      <c r="A454" s="69" t="s">
+      <c r="A454" s="68" t="s">
         <v>700</v>
       </c>
       <c r="B454" s="24">
@@ -13175,7 +13622,7 @@
       </c>
     </row>
     <row r="455" spans="1:6">
-      <c r="A455" s="69" t="s">
+      <c r="A455" s="68" t="s">
         <v>700</v>
       </c>
       <c r="B455" s="24">
@@ -13192,7 +13639,7 @@
       </c>
     </row>
     <row r="456" spans="1:6">
-      <c r="A456" s="69" t="s">
+      <c r="A456" s="68" t="s">
         <v>704</v>
       </c>
       <c r="B456" s="24">
@@ -13209,7 +13656,7 @@
       </c>
     </row>
     <row r="457" spans="1:6">
-      <c r="A457" s="69" t="s">
+      <c r="A457" s="68" t="s">
         <v>706</v>
       </c>
       <c r="B457" s="24">
@@ -13226,7 +13673,7 @@
       </c>
     </row>
     <row r="458" spans="1:6">
-      <c r="A458" s="69" t="s">
+      <c r="A458" s="68" t="s">
         <v>708</v>
       </c>
       <c r="B458" s="24">
@@ -13243,7 +13690,7 @@
       </c>
     </row>
     <row r="459" spans="1:6">
-      <c r="A459" s="69" t="s">
+      <c r="A459" s="68" t="s">
         <v>81</v>
       </c>
       <c r="B459" s="24">
@@ -13260,7 +13707,7 @@
       </c>
     </row>
     <row r="460" spans="1:6">
-      <c r="A460" s="69" t="s">
+      <c r="A460" s="68" t="s">
         <v>127</v>
       </c>
       <c r="B460" s="24">
@@ -13277,7 +13724,7 @@
       </c>
     </row>
     <row r="461" spans="1:6">
-      <c r="A461" s="69" t="s">
+      <c r="A461" s="68" t="s">
         <v>65</v>
       </c>
       <c r="B461" s="24">
@@ -13294,7 +13741,7 @@
       </c>
     </row>
     <row r="462" spans="1:6">
-      <c r="A462" s="69" t="s">
+      <c r="A462" s="68" t="s">
         <v>59</v>
       </c>
       <c r="B462" s="23">
@@ -13311,7 +13758,7 @@
       </c>
     </row>
     <row r="463" spans="1:6">
-      <c r="A463" s="69" t="s">
+      <c r="A463" s="68" t="s">
         <v>712</v>
       </c>
       <c r="B463" s="23">
@@ -13358,84 +13805,965 @@
         <v>716</v>
       </c>
       <c r="E465" s="33"/>
-      <c r="F465" s="70">
+      <c r="F465" s="69">
         <v>45176</v>
       </c>
-      <c r="G465" s="71"/>
-      <c r="H465" s="72"/>
+      <c r="G465" s="70"/>
+      <c r="H465" s="71"/>
     </row>
     <row r="466" spans="1:8">
-      <c r="A466" s="60"/>
-      <c r="B466" s="22"/>
-      <c r="C466" s="22"/>
-      <c r="D466"/>
+      <c r="A466" t="s">
+        <v>63</v>
+      </c>
+      <c r="B466">
+        <v>2123</v>
+      </c>
+      <c r="C466">
+        <v>1701</v>
+      </c>
+      <c r="D466" t="s">
+        <v>732</v>
+      </c>
       <c r="E466" s="22"/>
-      <c r="F466" s="22"/>
-      <c r="G466" s="61"/>
-      <c r="H466" s="62"/>
+      <c r="F466" s="78">
+        <v>45147</v>
+      </c>
+      <c r="G466" s="60"/>
+      <c r="H466" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="467" spans="1:8">
-      <c r="D467"/>
+      <c r="A467" t="s">
+        <v>63</v>
+      </c>
+      <c r="B467">
+        <v>2118</v>
+      </c>
+      <c r="C467">
+        <v>2003</v>
+      </c>
+      <c r="D467" t="s">
+        <v>733</v>
+      </c>
+      <c r="F467" s="78">
+        <v>45147</v>
+      </c>
+      <c r="H467" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="468" spans="1:8">
-      <c r="D468"/>
+      <c r="A468" t="s">
+        <v>500</v>
+      </c>
+      <c r="B468">
+        <v>2118</v>
+      </c>
+      <c r="C468">
+        <v>2304</v>
+      </c>
+      <c r="D468" t="s">
+        <v>734</v>
+      </c>
+      <c r="F468" s="78">
+        <v>45147</v>
+      </c>
+      <c r="H468" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="469" spans="1:8">
-      <c r="D469"/>
-    </row>
-    <row r="470" spans="1:8">
-      <c r="D470"/>
+      <c r="A469" t="s">
+        <v>63</v>
+      </c>
+      <c r="B469">
+        <v>2120</v>
+      </c>
+      <c r="C469">
+        <v>401</v>
+      </c>
+      <c r="D469" t="s">
+        <v>242</v>
+      </c>
+      <c r="F469" s="78">
+        <v>45147</v>
+      </c>
+      <c r="H469" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="470" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A470" t="s">
+        <v>63</v>
+      </c>
+      <c r="B470">
+        <v>2121</v>
+      </c>
+      <c r="C470">
+        <v>901</v>
+      </c>
+      <c r="D470" t="s">
+        <v>735</v>
+      </c>
+      <c r="F470" s="78">
+        <v>45147</v>
+      </c>
+      <c r="H470" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="471" spans="1:8">
-      <c r="D471"/>
+      <c r="A471" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B471" s="29" t="s">
+        <v>737</v>
+      </c>
+      <c r="C471" s="29" t="s">
+        <v>738</v>
+      </c>
+      <c r="D471" s="29" t="s">
+        <v>699</v>
+      </c>
+      <c r="F471" s="18">
+        <v>45180</v>
+      </c>
+      <c r="H471" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="472" spans="1:8">
-      <c r="D472"/>
+      <c r="A472" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B472" s="24" t="s">
+        <v>737</v>
+      </c>
+      <c r="C472" s="24" t="s">
+        <v>739</v>
+      </c>
+      <c r="D472" s="24" t="s">
+        <v>740</v>
+      </c>
+      <c r="F472" s="18">
+        <v>45180</v>
+      </c>
+      <c r="H472" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="473" spans="1:8">
-      <c r="D473"/>
+      <c r="A473" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B473" s="24" t="s">
+        <v>737</v>
+      </c>
+      <c r="C473" s="24" t="s">
+        <v>741</v>
+      </c>
+      <c r="D473" s="24" t="s">
+        <v>742</v>
+      </c>
+      <c r="F473" s="18">
+        <v>45180</v>
+      </c>
+      <c r="H473" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="474" spans="1:8">
-      <c r="D474"/>
+      <c r="A474" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B474" s="24" t="s">
+        <v>737</v>
+      </c>
+      <c r="C474" s="24" t="s">
+        <v>743</v>
+      </c>
+      <c r="D474" s="24" t="s">
+        <v>701</v>
+      </c>
+      <c r="F474" s="18">
+        <v>45180</v>
+      </c>
+      <c r="H474" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="475" spans="1:8">
-      <c r="D475"/>
+      <c r="A475" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B475" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="C475" s="24" t="s">
+        <v>745</v>
+      </c>
+      <c r="D475" s="24" t="s">
+        <v>746</v>
+      </c>
+      <c r="F475" s="18">
+        <v>45180</v>
+      </c>
+      <c r="H475" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="476" spans="1:8">
-      <c r="D476"/>
+      <c r="A476" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B476" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="C476" s="24" t="s">
+        <v>747</v>
+      </c>
+      <c r="D476" s="24" t="s">
+        <v>748</v>
+      </c>
+      <c r="F476" s="18">
+        <v>45180</v>
+      </c>
+      <c r="H476" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="477" spans="1:8">
-      <c r="D477"/>
+      <c r="A477" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B477" s="24" t="s">
+        <v>744</v>
+      </c>
+      <c r="C477" s="24" t="s">
+        <v>749</v>
+      </c>
+      <c r="D477" s="24" t="s">
+        <v>750</v>
+      </c>
+      <c r="F477" s="18">
+        <v>45180</v>
+      </c>
+      <c r="H477" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="478" spans="1:8">
-      <c r="D478"/>
+      <c r="A478" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B478" s="24" t="s">
+        <v>751</v>
+      </c>
+      <c r="C478" s="24" t="s">
+        <v>752</v>
+      </c>
+      <c r="D478" s="24" t="s">
+        <v>753</v>
+      </c>
+      <c r="F478" s="18">
+        <v>45180</v>
+      </c>
+      <c r="H478" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="479" spans="1:8">
-      <c r="D479"/>
+      <c r="A479" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B479" s="24" t="s">
+        <v>754</v>
+      </c>
+      <c r="C479" s="24" t="s">
+        <v>755</v>
+      </c>
+      <c r="D479" s="24" t="s">
+        <v>756</v>
+      </c>
+      <c r="F479" s="18">
+        <v>45180</v>
+      </c>
+      <c r="H479" s="61" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="480" spans="1:8">
-      <c r="D480" s="24"/>
-    </row>
-    <row r="481" spans="4:4">
-      <c r="D481" s="24"/>
-    </row>
-    <row r="482" spans="4:4">
-      <c r="D482" s="24"/>
-    </row>
-    <row r="483" spans="4:4">
-      <c r="D483"/>
-    </row>
-    <row r="484" spans="4:4">
-      <c r="D484"/>
-    </row>
-    <row r="485" spans="4:4">
-      <c r="D485"/>
-    </row>
-    <row r="486" spans="4:4">
-      <c r="D486"/>
-    </row>
-    <row r="487" spans="4:4">
-      <c r="D487"/>
+      <c r="A480" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B480" s="24" t="s">
+        <v>754</v>
+      </c>
+      <c r="C480" s="24" t="s">
+        <v>757</v>
+      </c>
+      <c r="D480" s="24" t="s">
+        <v>758</v>
+      </c>
+      <c r="F480" s="18">
+        <v>45180</v>
+      </c>
+      <c r="H480" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="481" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A481" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="B481" s="28" t="s">
+        <v>754</v>
+      </c>
+      <c r="C481" s="28" t="s">
+        <v>759</v>
+      </c>
+      <c r="D481" s="28" t="s">
+        <v>515</v>
+      </c>
+      <c r="F481" s="18">
+        <v>45180</v>
+      </c>
+      <c r="H481" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="482" spans="1:8">
+      <c r="A482" s="80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B482" s="81">
+        <v>101</v>
+      </c>
+      <c r="C482" s="81">
+        <v>602</v>
+      </c>
+      <c r="D482" s="80" t="s">
+        <v>760</v>
+      </c>
+      <c r="F482" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H482" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="483" spans="1:8">
+      <c r="A483" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B483" s="83">
+        <v>101</v>
+      </c>
+      <c r="C483" s="83">
+        <v>1001</v>
+      </c>
+      <c r="D483" s="83" t="s">
+        <v>761</v>
+      </c>
+      <c r="F483" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H483" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="484" spans="1:8">
+      <c r="A484" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B484" s="83">
+        <v>102</v>
+      </c>
+      <c r="C484" s="83">
+        <v>103</v>
+      </c>
+      <c r="D484" s="83" t="s">
+        <v>762</v>
+      </c>
+      <c r="F484" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H484" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="485" spans="1:8">
+      <c r="A485" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B485" s="83">
+        <v>102</v>
+      </c>
+      <c r="C485" s="83">
+        <v>201</v>
+      </c>
+      <c r="D485" s="84" t="s">
+        <v>763</v>
+      </c>
+      <c r="F485" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H485" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="486" spans="1:8">
+      <c r="A486" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B486" s="83">
+        <v>102</v>
+      </c>
+      <c r="C486" s="83">
+        <v>901</v>
+      </c>
+      <c r="D486" s="83" t="s">
+        <v>764</v>
+      </c>
+      <c r="F486" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H486" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="487" spans="1:8">
+      <c r="A487" s="85" t="s">
+        <v>67</v>
+      </c>
+      <c r="B487" s="86">
+        <v>102</v>
+      </c>
+      <c r="C487" s="86">
+        <v>1303</v>
+      </c>
+      <c r="D487" s="85" t="s">
+        <v>765</v>
+      </c>
+      <c r="F487" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H487" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="488" spans="1:8">
+      <c r="A488" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B488" s="83">
+        <v>103</v>
+      </c>
+      <c r="C488" s="83">
+        <v>901</v>
+      </c>
+      <c r="D488" s="83" t="s">
+        <v>766</v>
+      </c>
+      <c r="F488" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H488" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="489" spans="1:8">
+      <c r="A489" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="B489" s="88">
+        <v>104</v>
+      </c>
+      <c r="C489" s="88">
+        <v>803</v>
+      </c>
+      <c r="D489" s="88" t="s">
+        <v>767</v>
+      </c>
+      <c r="F489" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H489" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="490" spans="1:8">
+      <c r="A490" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B490" s="83">
+        <v>104</v>
+      </c>
+      <c r="C490" s="83">
+        <v>1506</v>
+      </c>
+      <c r="D490" s="83" t="s">
+        <v>768</v>
+      </c>
+      <c r="F490" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H490" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="491" spans="1:8">
+      <c r="A491" s="85" t="s">
+        <v>67</v>
+      </c>
+      <c r="B491" s="86">
+        <v>106</v>
+      </c>
+      <c r="C491" s="86">
+        <v>1303</v>
+      </c>
+      <c r="D491" s="86" t="s">
+        <v>769</v>
+      </c>
+      <c r="F491" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H491" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="492" spans="1:8">
+      <c r="A492" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B492" s="83">
+        <v>106</v>
+      </c>
+      <c r="C492" s="83">
+        <v>1505</v>
+      </c>
+      <c r="D492" s="83" t="s">
+        <v>770</v>
+      </c>
+      <c r="F492" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H492" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="493" spans="1:8">
+      <c r="A493" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B493" s="83">
+        <v>107</v>
+      </c>
+      <c r="C493" s="83">
+        <v>802</v>
+      </c>
+      <c r="D493" s="83" t="s">
+        <v>771</v>
+      </c>
+      <c r="F493" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H493" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="494" spans="1:8">
+      <c r="A494" s="85" t="s">
+        <v>67</v>
+      </c>
+      <c r="B494" s="86">
+        <v>107</v>
+      </c>
+      <c r="C494" s="86">
+        <v>1001</v>
+      </c>
+      <c r="D494" s="86" t="s">
+        <v>772</v>
+      </c>
+      <c r="F494" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H494" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="495" spans="1:8">
+      <c r="A495" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B495" s="83">
+        <v>107</v>
+      </c>
+      <c r="C495" s="83">
+        <v>1101</v>
+      </c>
+      <c r="D495" s="83" t="s">
+        <v>773</v>
+      </c>
+      <c r="F495" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H495" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="496" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A496" s="89" t="s">
+        <v>67</v>
+      </c>
+      <c r="B496" s="90">
+        <v>107</v>
+      </c>
+      <c r="C496" s="90">
+        <v>1304</v>
+      </c>
+      <c r="D496" s="89" t="s">
+        <v>774</v>
+      </c>
+      <c r="F496" s="18">
+        <v>45163</v>
+      </c>
+      <c r="H496" s="61" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="497" spans="1:6">
+      <c r="A497" s="20" t="s">
+        <v>831</v>
+      </c>
+      <c r="B497" s="19">
+        <v>101</v>
+      </c>
+      <c r="C497" s="19">
+        <v>406</v>
+      </c>
+      <c r="D497" s="19" t="s">
+        <v>775</v>
+      </c>
+      <c r="F497" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="498" spans="1:6">
+      <c r="A498" s="20" t="s">
+        <v>832</v>
+      </c>
+      <c r="B498" s="19">
+        <v>312</v>
+      </c>
+      <c r="C498" s="19">
+        <v>1308</v>
+      </c>
+      <c r="D498" t="s">
+        <v>776</v>
+      </c>
+      <c r="F498" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="499" spans="1:6">
+      <c r="A499" s="20" t="s">
+        <v>832</v>
+      </c>
+      <c r="B499" s="19">
+        <v>918</v>
+      </c>
+      <c r="C499" s="19">
+        <v>903</v>
+      </c>
+      <c r="D499" t="s">
+        <v>777</v>
+      </c>
+      <c r="F499" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="500" spans="1:6">
+      <c r="A500" s="20" t="s">
+        <v>833</v>
+      </c>
+      <c r="B500" s="19">
+        <v>102</v>
+      </c>
+      <c r="C500" s="19">
+        <v>1205</v>
+      </c>
+      <c r="D500" s="91" t="s">
+        <v>782</v>
+      </c>
+      <c r="F500" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="501" spans="1:6">
+      <c r="A501" s="20" t="s">
+        <v>834</v>
+      </c>
+      <c r="B501" s="19">
+        <v>101</v>
+      </c>
+      <c r="C501" s="19">
+        <v>508</v>
+      </c>
+      <c r="D501" t="s">
+        <v>784</v>
+      </c>
+      <c r="F501" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="502" spans="1:6">
+      <c r="A502" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="B502" s="19">
+        <v>106</v>
+      </c>
+      <c r="C502" s="19">
+        <v>1301</v>
+      </c>
+      <c r="D502" t="s">
+        <v>783</v>
+      </c>
+      <c r="F502" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="503" spans="1:6">
+      <c r="A503" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="B503" s="19">
+        <v>117</v>
+      </c>
+      <c r="C503" s="19">
+        <v>903</v>
+      </c>
+      <c r="D503" t="s">
+        <v>792</v>
+      </c>
+      <c r="F503" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="504" spans="1:6">
+      <c r="A504" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B504" s="19">
+        <v>104</v>
+      </c>
+      <c r="C504" s="19">
+        <v>1503</v>
+      </c>
+      <c r="D504" t="s">
+        <v>788</v>
+      </c>
+      <c r="F504" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="505" spans="1:6">
+      <c r="A505" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B505" s="19">
+        <v>105</v>
+      </c>
+      <c r="C505" s="19">
+        <v>903</v>
+      </c>
+      <c r="D505" t="s">
+        <v>787</v>
+      </c>
+      <c r="F505" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="506" spans="1:6">
+      <c r="A506" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B506" s="19">
+        <v>107</v>
+      </c>
+      <c r="C506" s="19">
+        <v>103</v>
+      </c>
+      <c r="D506" t="s">
+        <v>830</v>
+      </c>
+      <c r="F506" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6">
+      <c r="A507" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B507" s="19">
+        <v>108</v>
+      </c>
+      <c r="C507" s="19">
+        <v>1403</v>
+      </c>
+      <c r="D507" t="s">
+        <v>785</v>
+      </c>
+      <c r="F507" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6">
+      <c r="A508" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B508" s="19">
+        <v>109</v>
+      </c>
+      <c r="C508" s="19">
+        <v>1005</v>
+      </c>
+      <c r="D508" t="s">
+        <v>786</v>
+      </c>
+      <c r="F508" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6">
+      <c r="A509" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B509" s="19">
+        <v>109</v>
+      </c>
+      <c r="C509" s="19">
+        <v>1003</v>
+      </c>
+      <c r="D509" t="s">
+        <v>791</v>
+      </c>
+      <c r="F509" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6">
+      <c r="A510" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B510" s="19">
+        <v>111</v>
+      </c>
+      <c r="C510" s="19">
+        <v>1303</v>
+      </c>
+      <c r="D510" t="s">
+        <v>790</v>
+      </c>
+      <c r="F510" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6">
+      <c r="A511" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B511" s="19">
+        <v>126</v>
+      </c>
+      <c r="C511" s="19">
+        <v>1107</v>
+      </c>
+      <c r="D511" t="s">
+        <v>789</v>
+      </c>
+      <c r="F511" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6">
+      <c r="A512" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B512" s="19">
+        <v>103</v>
+      </c>
+      <c r="C512" s="19">
+        <v>801</v>
+      </c>
+      <c r="D512" t="s">
+        <v>780</v>
+      </c>
+      <c r="F512" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6">
+      <c r="A513" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B513" s="19">
+        <v>111</v>
+      </c>
+      <c r="C513" s="19">
+        <v>801</v>
+      </c>
+      <c r="D513" t="s">
+        <v>779</v>
+      </c>
+      <c r="F513" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6">
+      <c r="A514" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B514" s="19">
+        <v>116</v>
+      </c>
+      <c r="C514" s="19">
+        <v>501</v>
+      </c>
+      <c r="D514" t="s">
+        <v>778</v>
+      </c>
+      <c r="F514" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6">
+      <c r="A515" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B515" s="19">
+        <v>122</v>
+      </c>
+      <c r="C515" s="19">
+        <v>701</v>
+      </c>
+      <c r="D515" t="s">
+        <v>781</v>
+      </c>
+      <c r="F515" s="18">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6">
+      <c r="D516"/>
+    </row>
+    <row r="517" spans="1:6">
+      <c r="D517"/>
+    </row>
+    <row r="518" spans="1:6">
+      <c r="D518"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -13450,173 +14778,188 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D3:D396 D398:D451 D464:D487">
-    <cfRule type="duplicateValues" dxfId="73" priority="5"/>
+  <conditionalFormatting sqref="D3:D396 D398:D451 D464:D470">
+    <cfRule type="duplicateValues" dxfId="79" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D396 D398:D451">
-    <cfRule type="duplicateValues" dxfId="72" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D518">
+    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D397">
-    <cfRule type="duplicateValues" dxfId="71" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D454">
-    <cfRule type="duplicateValues" dxfId="70" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D455">
-    <cfRule type="duplicateValues" dxfId="69" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D456">
-    <cfRule type="duplicateValues" dxfId="68" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D464">
-    <cfRule type="duplicateValues" dxfId="67" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D465:D466">
-    <cfRule type="duplicateValues" dxfId="66" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D467:D469">
-    <cfRule type="duplicateValues" dxfId="65" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D470:D479">
-    <cfRule type="duplicateValues" dxfId="64" priority="7"/>
+  <conditionalFormatting sqref="D470">
+    <cfRule type="duplicateValues" dxfId="69" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D480:D487">
-    <cfRule type="duplicateValues" dxfId="63" priority="6"/>
+  <conditionalFormatting sqref="D473">
+    <cfRule type="duplicateValues" dxfId="68" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D474">
+    <cfRule type="duplicateValues" dxfId="67" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D482:D493">
+    <cfRule type="duplicateValues" dxfId="66" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D498:D518">
+    <cfRule type="duplicateValues" dxfId="65" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D501:D514">
+    <cfRule type="duplicateValues" dxfId="64" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18:E18">
-    <cfRule type="duplicateValues" dxfId="62" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:E20">
-    <cfRule type="duplicateValues" dxfId="61" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="64"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:E21">
-    <cfRule type="duplicateValues" dxfId="60" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:E22">
-    <cfRule type="duplicateValues" dxfId="59" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="62"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:E23">
-    <cfRule type="duplicateValues" dxfId="58" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:E24">
-    <cfRule type="duplicateValues" dxfId="57" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:E25">
-    <cfRule type="duplicateValues" dxfId="56" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:E26">
-    <cfRule type="duplicateValues" dxfId="55" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="58"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:E27">
-    <cfRule type="duplicateValues" dxfId="54" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:E28">
-    <cfRule type="duplicateValues" dxfId="53" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:E29">
-    <cfRule type="duplicateValues" dxfId="52" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30:E30">
-    <cfRule type="duplicateValues" dxfId="51" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:E31">
-    <cfRule type="duplicateValues" dxfId="50" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:E32">
-    <cfRule type="duplicateValues" dxfId="49" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:E33">
-    <cfRule type="duplicateValues" dxfId="48" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:E34">
-    <cfRule type="duplicateValues" dxfId="47" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:E35">
-    <cfRule type="duplicateValues" dxfId="46" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36:E36">
-    <cfRule type="duplicateValues" dxfId="45" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:E41">
-    <cfRule type="duplicateValues" dxfId="44" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D42:E42">
-    <cfRule type="duplicateValues" dxfId="43" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:E43">
-    <cfRule type="duplicateValues" dxfId="42" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44:E44">
-    <cfRule type="duplicateValues" dxfId="41" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:E45">
-    <cfRule type="duplicateValues" dxfId="40" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46:E46">
-    <cfRule type="duplicateValues" dxfId="39" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47:E47">
-    <cfRule type="duplicateValues" dxfId="38" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48:E56">
-    <cfRule type="duplicateValues" dxfId="37" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57:E57">
-    <cfRule type="duplicateValues" dxfId="36" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58:E68">
-    <cfRule type="duplicateValues" dxfId="35" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:E83">
-    <cfRule type="duplicateValues" dxfId="34" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D84:E85">
-    <cfRule type="duplicateValues" dxfId="33" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87:E87">
-    <cfRule type="duplicateValues" dxfId="32" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D102:E102">
-    <cfRule type="duplicateValues" dxfId="31" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D103:E103">
-    <cfRule type="duplicateValues" dxfId="30" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D104:E104">
-    <cfRule type="duplicateValues" dxfId="29" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D105:E105">
-    <cfRule type="duplicateValues" dxfId="28" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106:E106">
-    <cfRule type="duplicateValues" dxfId="27" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108:E108">
-    <cfRule type="duplicateValues" dxfId="26" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110:E110">
-    <cfRule type="duplicateValues" dxfId="25" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D112:E112">
-    <cfRule type="duplicateValues" dxfId="24" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D113:E113">
-    <cfRule type="duplicateValues" dxfId="23" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D114:E114">
-    <cfRule type="duplicateValues" dxfId="22" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D115:E115">
-    <cfRule type="duplicateValues" dxfId="21" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D116:E116 D111:E111 D118:E118 D109:E109 D107:E107">
-    <cfRule type="duplicateValues" dxfId="20" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D117:E117">
-    <cfRule type="duplicateValues" dxfId="19" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D149:E149">
-    <cfRule type="duplicateValues" dxfId="18" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="21"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -13625,10 +14968,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2252FB-561C-4694-B5F3-846A13872E41}">
-  <dimension ref="A1:M205"/>
+  <dimension ref="A1:M202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -13720,7 +15063,7 @@
       <c r="K2" s="46" t="s">
         <v>585</v>
       </c>
-      <c r="L2" s="85" t="s">
+      <c r="L2" s="99" t="s">
         <v>586</v>
       </c>
       <c r="M2" s="51" t="s">
@@ -13757,7 +15100,7 @@
       <c r="K3" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L3" s="84"/>
+      <c r="L3" s="98"/>
       <c r="M3" s="48" t="s">
         <v>392</v>
       </c>
@@ -13796,7 +15139,7 @@
       <c r="K4" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L4" s="84"/>
+      <c r="L4" s="98"/>
       <c r="M4" s="48" t="s">
         <v>392</v>
       </c>
@@ -13831,7 +15174,7 @@
       <c r="K5" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L5" s="84"/>
+      <c r="L5" s="98"/>
       <c r="M5" s="48" t="s">
         <v>392</v>
       </c>
@@ -13870,7 +15213,7 @@
       <c r="K6" s="24" t="s">
         <v>585</v>
       </c>
-      <c r="L6" s="84"/>
+      <c r="L6" s="98"/>
       <c r="M6" s="52" t="s">
         <v>393</v>
       </c>
@@ -13899,7 +15242,7 @@
       </c>
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
-      <c r="L7" s="84"/>
+      <c r="L7" s="98"/>
       <c r="M7" s="48" t="s">
         <v>394</v>
       </c>
@@ -13928,7 +15271,7 @@
       </c>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
-      <c r="L8" s="84"/>
+      <c r="L8" s="98"/>
       <c r="M8" s="48" t="s">
         <v>395</v>
       </c>
@@ -13957,7 +15300,7 @@
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
-      <c r="L9" s="84"/>
+      <c r="L9" s="98"/>
       <c r="M9" s="48" t="s">
         <v>396</v>
       </c>
@@ -13990,7 +15333,7 @@
       </c>
       <c r="J10" s="24"/>
       <c r="K10" s="24"/>
-      <c r="L10" s="84"/>
+      <c r="L10" s="98"/>
       <c r="M10" s="48" t="s">
         <v>397</v>
       </c>
@@ -14019,7 +15362,7 @@
       </c>
       <c r="J11" s="24"/>
       <c r="K11" s="24"/>
-      <c r="L11" s="83" t="s">
+      <c r="L11" s="97" t="s">
         <v>593</v>
       </c>
       <c r="M11" s="48" t="s">
@@ -14050,7 +15393,7 @@
       </c>
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
-      <c r="L12" s="83"/>
+      <c r="L12" s="97"/>
       <c r="M12" s="48" t="s">
         <v>398</v>
       </c>
@@ -14079,7 +15422,7 @@
       </c>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
-      <c r="L13" s="83"/>
+      <c r="L13" s="97"/>
       <c r="M13" s="48" t="s">
         <v>398</v>
       </c>
@@ -14108,7 +15451,7 @@
       </c>
       <c r="J14" s="24"/>
       <c r="K14" s="24"/>
-      <c r="L14" s="83"/>
+      <c r="L14" s="97"/>
       <c r="M14" s="48" t="s">
         <v>398</v>
       </c>
@@ -14137,7 +15480,7 @@
       </c>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
-      <c r="L15" s="83"/>
+      <c r="L15" s="97"/>
       <c r="M15" s="48" t="s">
         <v>399</v>
       </c>
@@ -14166,7 +15509,7 @@
       </c>
       <c r="J16" s="24"/>
       <c r="K16" s="24"/>
-      <c r="L16" s="83"/>
+      <c r="L16" s="97"/>
       <c r="M16" s="48" t="s">
         <v>400</v>
       </c>
@@ -14195,7 +15538,7 @@
       </c>
       <c r="J17" s="24"/>
       <c r="K17" s="24"/>
-      <c r="L17" s="83"/>
+      <c r="L17" s="97"/>
       <c r="M17" s="48" t="s">
         <v>400</v>
       </c>
@@ -14224,7 +15567,7 @@
       </c>
       <c r="J18" s="24"/>
       <c r="K18" s="24"/>
-      <c r="L18" s="83"/>
+      <c r="L18" s="97"/>
       <c r="M18" s="48" t="s">
         <v>401</v>
       </c>
@@ -14253,7 +15596,7 @@
       </c>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
-      <c r="L19" s="83"/>
+      <c r="L19" s="97"/>
       <c r="M19" s="48" t="s">
         <v>402</v>
       </c>
@@ -14282,7 +15625,7 @@
       </c>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
-      <c r="L20" s="83"/>
+      <c r="L20" s="97"/>
       <c r="M20" s="48" t="s">
         <v>403</v>
       </c>
@@ -14311,7 +15654,7 @@
       </c>
       <c r="J21" s="24"/>
       <c r="K21" s="24"/>
-      <c r="L21" s="83"/>
+      <c r="L21" s="97"/>
       <c r="M21" s="48" t="s">
         <v>403</v>
       </c>
@@ -14350,7 +15693,7 @@
       <c r="K22" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L22" s="84" t="s">
+      <c r="L22" s="98" t="s">
         <v>595</v>
       </c>
       <c r="M22" s="48" t="s">
@@ -14391,7 +15734,7 @@
       <c r="K23" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L23" s="84"/>
+      <c r="L23" s="98"/>
       <c r="M23" s="48" t="s">
         <v>404</v>
       </c>
@@ -14430,7 +15773,7 @@
       <c r="K24" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L24" s="84"/>
+      <c r="L24" s="98"/>
       <c r="M24" s="48" t="s">
         <v>405</v>
       </c>
@@ -14469,7 +15812,7 @@
       <c r="K25" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L25" s="84"/>
+      <c r="L25" s="98"/>
       <c r="M25" s="48" t="s">
         <v>406</v>
       </c>
@@ -14508,7 +15851,7 @@
       <c r="K26" s="41" t="s">
         <v>601</v>
       </c>
-      <c r="L26" s="84"/>
+      <c r="L26" s="98"/>
       <c r="M26" s="48" t="s">
         <v>407</v>
       </c>
@@ -14545,7 +15888,7 @@
       <c r="K27" s="41" t="s">
         <v>601</v>
       </c>
-      <c r="L27" s="84"/>
+      <c r="L27" s="98"/>
       <c r="M27" s="48" t="s">
         <v>407</v>
       </c>
@@ -14580,7 +15923,7 @@
       </c>
       <c r="J28" s="24"/>
       <c r="K28" s="24"/>
-      <c r="L28" s="84"/>
+      <c r="L28" s="98"/>
       <c r="M28" s="48" t="s">
         <v>408</v>
       </c>
@@ -14615,7 +15958,7 @@
       </c>
       <c r="J29" s="24"/>
       <c r="K29" s="24"/>
-      <c r="L29" s="84"/>
+      <c r="L29" s="98"/>
       <c r="M29" s="48" t="s">
         <v>408</v>
       </c>
@@ -14650,7 +15993,7 @@
       </c>
       <c r="J30" s="24"/>
       <c r="K30" s="24"/>
-      <c r="L30" s="84"/>
+      <c r="L30" s="98"/>
       <c r="M30" s="48" t="s">
         <v>409</v>
       </c>
@@ -14681,7 +16024,7 @@
       <c r="I31" s="24"/>
       <c r="J31" s="24"/>
       <c r="K31" s="24"/>
-      <c r="L31" s="84"/>
+      <c r="L31" s="98"/>
       <c r="M31" s="48" t="s">
         <v>410</v>
       </c>
@@ -14712,7 +16055,7 @@
       <c r="I32" s="24"/>
       <c r="J32" s="24"/>
       <c r="K32" s="24"/>
-      <c r="L32" s="84"/>
+      <c r="L32" s="98"/>
       <c r="M32" s="48" t="s">
         <v>410</v>
       </c>
@@ -14745,7 +16088,7 @@
       </c>
       <c r="J33" s="24"/>
       <c r="K33" s="24"/>
-      <c r="L33" s="84"/>
+      <c r="L33" s="98"/>
       <c r="M33" s="48" t="s">
         <v>410</v>
       </c>
@@ -14772,7 +16115,7 @@
       <c r="I34" s="24"/>
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
-      <c r="L34" s="84"/>
+      <c r="L34" s="98"/>
       <c r="M34" s="48" t="s">
         <v>410</v>
       </c>
@@ -14811,7 +16154,7 @@
       <c r="K35" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L35" s="84" t="s">
+      <c r="L35" s="98" t="s">
         <v>610</v>
       </c>
       <c r="M35" s="48" t="s">
@@ -14822,7 +16165,7 @@
       <c r="A36" s="47">
         <v>35</v>
       </c>
-      <c r="B36" s="83" t="s">
+      <c r="B36" s="97" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="24">
@@ -14846,7 +16189,7 @@
       <c r="K36" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L36" s="84"/>
+      <c r="L36" s="98"/>
       <c r="M36" s="48" t="s">
         <v>412</v>
       </c>
@@ -14855,7 +16198,7 @@
       <c r="A37" s="47">
         <v>36</v>
       </c>
-      <c r="B37" s="83"/>
+      <c r="B37" s="97"/>
       <c r="C37" s="24">
         <v>101</v>
       </c>
@@ -14877,7 +16220,7 @@
       <c r="K37" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L37" s="84"/>
+      <c r="L37" s="98"/>
       <c r="M37" s="48" t="s">
         <v>413</v>
       </c>
@@ -14886,7 +16229,7 @@
       <c r="A38" s="47">
         <v>37</v>
       </c>
-      <c r="B38" s="83"/>
+      <c r="B38" s="97"/>
       <c r="C38" s="24">
         <v>101</v>
       </c>
@@ -14914,7 +16257,7 @@
       <c r="K38" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L38" s="84"/>
+      <c r="L38" s="98"/>
       <c r="M38" s="48" t="s">
         <v>413</v>
       </c>
@@ -14923,7 +16266,7 @@
       <c r="A39" s="47">
         <v>38</v>
       </c>
-      <c r="B39" s="83"/>
+      <c r="B39" s="97"/>
       <c r="C39" s="24">
         <v>101</v>
       </c>
@@ -14951,7 +16294,7 @@
       <c r="K39" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L39" s="84"/>
+      <c r="L39" s="98"/>
       <c r="M39" s="48" t="s">
         <v>413</v>
       </c>
@@ -14960,7 +16303,7 @@
       <c r="A40" s="47">
         <v>39</v>
       </c>
-      <c r="B40" s="83"/>
+      <c r="B40" s="97"/>
       <c r="C40" s="24">
         <v>101</v>
       </c>
@@ -14982,7 +16325,7 @@
       <c r="K40" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L40" s="84"/>
+      <c r="L40" s="98"/>
       <c r="M40" s="53" t="s">
         <v>414</v>
       </c>
@@ -14991,7 +16334,7 @@
       <c r="A41" s="47">
         <v>40</v>
       </c>
-      <c r="B41" s="83"/>
+      <c r="B41" s="97"/>
       <c r="C41" s="24">
         <v>125</v>
       </c>
@@ -15011,7 +16354,7 @@
       <c r="K41" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L41" s="84"/>
+      <c r="L41" s="98"/>
       <c r="M41" s="48" t="s">
         <v>415</v>
       </c>
@@ -15020,7 +16363,7 @@
       <c r="A42" s="47">
         <v>41</v>
       </c>
-      <c r="B42" s="83"/>
+      <c r="B42" s="97"/>
       <c r="C42" s="24">
         <v>102</v>
       </c>
@@ -15042,7 +16385,7 @@
       <c r="K42" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L42" s="84"/>
+      <c r="L42" s="98"/>
       <c r="M42" s="48" t="s">
         <v>416</v>
       </c>
@@ -15051,7 +16394,7 @@
       <c r="A43" s="47">
         <v>42</v>
       </c>
-      <c r="B43" s="83"/>
+      <c r="B43" s="97"/>
       <c r="C43" s="24">
         <v>123</v>
       </c>
@@ -15073,7 +16416,7 @@
       <c r="K43" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L43" s="84"/>
+      <c r="L43" s="98"/>
       <c r="M43" s="48" t="s">
         <v>417</v>
       </c>
@@ -15082,7 +16425,7 @@
       <c r="A44" s="47">
         <v>43</v>
       </c>
-      <c r="B44" s="83"/>
+      <c r="B44" s="97"/>
       <c r="C44" s="24">
         <v>115</v>
       </c>
@@ -15104,7 +16447,7 @@
       <c r="K44" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L44" s="84"/>
+      <c r="L44" s="98"/>
       <c r="M44" s="48" t="s">
         <v>418</v>
       </c>
@@ -15113,7 +16456,7 @@
       <c r="A45" s="47">
         <v>44</v>
       </c>
-      <c r="B45" s="83"/>
+      <c r="B45" s="97"/>
       <c r="C45" s="24">
         <v>105</v>
       </c>
@@ -15135,7 +16478,7 @@
       <c r="K45" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L45" s="84"/>
+      <c r="L45" s="98"/>
       <c r="M45" s="48" t="s">
         <v>419</v>
       </c>
@@ -15144,7 +16487,7 @@
       <c r="A46" s="47">
         <v>45</v>
       </c>
-      <c r="B46" s="83"/>
+      <c r="B46" s="97"/>
       <c r="C46" s="24">
         <v>106</v>
       </c>
@@ -15166,7 +16509,7 @@
       <c r="K46" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L46" s="84"/>
+      <c r="L46" s="98"/>
       <c r="M46" s="48" t="s">
         <v>419</v>
       </c>
@@ -15175,7 +16518,7 @@
       <c r="A47" s="47">
         <v>46</v>
       </c>
-      <c r="B47" s="83"/>
+      <c r="B47" s="97"/>
       <c r="C47" s="24">
         <v>106</v>
       </c>
@@ -15197,7 +16540,7 @@
       <c r="K47" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L47" s="84"/>
+      <c r="L47" s="98"/>
       <c r="M47" s="48" t="s">
         <v>419</v>
       </c>
@@ -15206,7 +16549,7 @@
       <c r="A48" s="47">
         <v>47</v>
       </c>
-      <c r="B48" s="83"/>
+      <c r="B48" s="97"/>
       <c r="C48" s="24">
         <v>111</v>
       </c>
@@ -15234,7 +16577,7 @@
       <c r="K48" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L48" s="84"/>
+      <c r="L48" s="98"/>
       <c r="M48" s="48" t="s">
         <v>420</v>
       </c>
@@ -15243,7 +16586,7 @@
       <c r="A49" s="47">
         <v>48</v>
       </c>
-      <c r="B49" s="83"/>
+      <c r="B49" s="97"/>
       <c r="C49" s="24">
         <v>116</v>
       </c>
@@ -15265,7 +16608,7 @@
       <c r="K49" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L49" s="84"/>
+      <c r="L49" s="98"/>
       <c r="M49" s="48" t="s">
         <v>421</v>
       </c>
@@ -15274,7 +16617,7 @@
       <c r="A50" s="47">
         <v>49</v>
       </c>
-      <c r="B50" s="83"/>
+      <c r="B50" s="97"/>
       <c r="C50" s="24">
         <v>102</v>
       </c>
@@ -15296,7 +16639,7 @@
       <c r="K50" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L50" s="84"/>
+      <c r="L50" s="98"/>
       <c r="M50" s="48" t="s">
         <v>422</v>
       </c>
@@ -15329,7 +16672,7 @@
       <c r="K51" s="41" t="s">
         <v>601</v>
       </c>
-      <c r="L51" s="84"/>
+      <c r="L51" s="98"/>
       <c r="M51" s="48" t="s">
         <v>416</v>
       </c>
@@ -15362,7 +16705,7 @@
       <c r="K52" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L52" s="84"/>
+      <c r="L52" s="98"/>
       <c r="M52" s="48" t="s">
         <v>423</v>
       </c>
@@ -15401,7 +16744,7 @@
       <c r="K53" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L53" s="84"/>
+      <c r="L53" s="98"/>
       <c r="M53" s="48" t="s">
         <v>424</v>
       </c>
@@ -15440,7 +16783,7 @@
       <c r="K54" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L54" s="84"/>
+      <c r="L54" s="98"/>
       <c r="M54" s="48" t="s">
         <v>425</v>
       </c>
@@ -15479,7 +16822,7 @@
       <c r="K55" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L55" s="84"/>
+      <c r="L55" s="98"/>
       <c r="M55" s="48" t="s">
         <v>422</v>
       </c>
@@ -15518,7 +16861,7 @@
       <c r="K56" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L56" s="84"/>
+      <c r="L56" s="98"/>
       <c r="M56" s="48" t="s">
         <v>422</v>
       </c>
@@ -15547,7 +16890,7 @@
       </c>
       <c r="J57" s="24"/>
       <c r="K57" s="24"/>
-      <c r="L57" s="84"/>
+      <c r="L57" s="98"/>
       <c r="M57" s="48" t="s">
         <v>426</v>
       </c>
@@ -15576,7 +16919,7 @@
       </c>
       <c r="J58" s="24"/>
       <c r="K58" s="24"/>
-      <c r="L58" s="84"/>
+      <c r="L58" s="98"/>
       <c r="M58" s="48" t="s">
         <v>426</v>
       </c>
@@ -15605,7 +16948,7 @@
       </c>
       <c r="J59" s="24"/>
       <c r="K59" s="24"/>
-      <c r="L59" s="84"/>
+      <c r="L59" s="98"/>
       <c r="M59" s="48" t="s">
         <v>427</v>
       </c>
@@ -15640,7 +16983,7 @@
       </c>
       <c r="J60" s="24"/>
       <c r="K60" s="24"/>
-      <c r="L60" s="84"/>
+      <c r="L60" s="98"/>
       <c r="M60" s="48" t="s">
         <v>428</v>
       </c>
@@ -15675,7 +17018,7 @@
       </c>
       <c r="J61" s="24"/>
       <c r="K61" s="24"/>
-      <c r="L61" s="84"/>
+      <c r="L61" s="98"/>
       <c r="M61" s="48" t="s">
         <v>428</v>
       </c>
@@ -15710,7 +17053,7 @@
       </c>
       <c r="J62" s="24"/>
       <c r="K62" s="24"/>
-      <c r="L62" s="84"/>
+      <c r="L62" s="98"/>
       <c r="M62" s="48" t="s">
         <v>428</v>
       </c>
@@ -15745,7 +17088,7 @@
       </c>
       <c r="J63" s="24"/>
       <c r="K63" s="24"/>
-      <c r="L63" s="84"/>
+      <c r="L63" s="98"/>
       <c r="M63" s="48" t="s">
         <v>428</v>
       </c>
@@ -15774,7 +17117,7 @@
       </c>
       <c r="J64" s="24"/>
       <c r="K64" s="24"/>
-      <c r="L64" s="84"/>
+      <c r="L64" s="98"/>
       <c r="M64" s="48" t="s">
         <v>429</v>
       </c>
@@ -15803,7 +17146,7 @@
       </c>
       <c r="J65" s="24"/>
       <c r="K65" s="24"/>
-      <c r="L65" s="84"/>
+      <c r="L65" s="98"/>
       <c r="M65" s="48" t="s">
         <v>430</v>
       </c>
@@ -15830,7 +17173,7 @@
       </c>
       <c r="J66" s="24"/>
       <c r="K66" s="24"/>
-      <c r="L66" s="84"/>
+      <c r="L66" s="98"/>
       <c r="M66" s="48" t="s">
         <v>431</v>
       </c>
@@ -15857,7 +17200,7 @@
       </c>
       <c r="J67" s="24"/>
       <c r="K67" s="24"/>
-      <c r="L67" s="84"/>
+      <c r="L67" s="98"/>
       <c r="M67" s="48" t="s">
         <v>431</v>
       </c>
@@ -15884,7 +17227,7 @@
       </c>
       <c r="J68" s="24"/>
       <c r="K68" s="24"/>
-      <c r="L68" s="84"/>
+      <c r="L68" s="98"/>
       <c r="M68" s="48" t="s">
         <v>432</v>
       </c>
@@ -15913,7 +17256,7 @@
       </c>
       <c r="J69" s="24"/>
       <c r="K69" s="24"/>
-      <c r="L69" s="84"/>
+      <c r="L69" s="98"/>
       <c r="M69" s="48" t="s">
         <v>433</v>
       </c>
@@ -15942,7 +17285,7 @@
       </c>
       <c r="J70" s="24"/>
       <c r="K70" s="24"/>
-      <c r="L70" s="84"/>
+      <c r="L70" s="98"/>
       <c r="M70" s="48" t="s">
         <v>434</v>
       </c>
@@ -15971,7 +17314,7 @@
       </c>
       <c r="J71" s="24"/>
       <c r="K71" s="24"/>
-      <c r="L71" s="84"/>
+      <c r="L71" s="98"/>
       <c r="M71" s="48" t="s">
         <v>435</v>
       </c>
@@ -16000,7 +17343,7 @@
       </c>
       <c r="J72" s="24"/>
       <c r="K72" s="24"/>
-      <c r="L72" s="84"/>
+      <c r="L72" s="98"/>
       <c r="M72" s="48" t="s">
         <v>436</v>
       </c>
@@ -16029,7 +17372,7 @@
       </c>
       <c r="J73" s="24"/>
       <c r="K73" s="24"/>
-      <c r="L73" s="84"/>
+      <c r="L73" s="98"/>
       <c r="M73" s="48" t="s">
         <v>437</v>
       </c>
@@ -16058,7 +17401,7 @@
       </c>
       <c r="J74" s="24"/>
       <c r="K74" s="24"/>
-      <c r="L74" s="84"/>
+      <c r="L74" s="98"/>
       <c r="M74" s="48" t="s">
         <v>438</v>
       </c>
@@ -16087,7 +17430,7 @@
       </c>
       <c r="J75" s="24"/>
       <c r="K75" s="24"/>
-      <c r="L75" s="84"/>
+      <c r="L75" s="98"/>
       <c r="M75" s="48" t="s">
         <v>439</v>
       </c>
@@ -16116,7 +17459,7 @@
       </c>
       <c r="J76" s="24"/>
       <c r="K76" s="24"/>
-      <c r="L76" s="84"/>
+      <c r="L76" s="98"/>
       <c r="M76" s="48" t="s">
         <v>440</v>
       </c>
@@ -16155,7 +17498,7 @@
       <c r="K77" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L77" s="84" t="s">
+      <c r="L77" s="98" t="s">
         <v>441</v>
       </c>
       <c r="M77" s="48" t="s">
@@ -16196,7 +17539,7 @@
       <c r="K78" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L78" s="84"/>
+      <c r="L78" s="98"/>
       <c r="M78" s="48" t="s">
         <v>442</v>
       </c>
@@ -16229,7 +17572,7 @@
       <c r="K79" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L79" s="84"/>
+      <c r="L79" s="98"/>
       <c r="M79" s="53" t="s">
         <v>443</v>
       </c>
@@ -16262,7 +17605,7 @@
       <c r="K80" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L80" s="84"/>
+      <c r="L80" s="98"/>
       <c r="M80" s="48" t="s">
         <v>444</v>
       </c>
@@ -16295,7 +17638,7 @@
       <c r="K81" s="41" t="s">
         <v>601</v>
       </c>
-      <c r="L81" s="84"/>
+      <c r="L81" s="98"/>
       <c r="M81" s="48" t="s">
         <v>445</v>
       </c>
@@ -16334,7 +17677,7 @@
       <c r="K82" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L82" s="84"/>
+      <c r="L82" s="98"/>
       <c r="M82" s="48" t="s">
         <v>446</v>
       </c>
@@ -16367,7 +17710,7 @@
       <c r="K83" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L83" s="84"/>
+      <c r="L83" s="98"/>
       <c r="M83" s="48" t="s">
         <v>447</v>
       </c>
@@ -16400,7 +17743,7 @@
       <c r="K84" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L84" s="84"/>
+      <c r="L84" s="98"/>
       <c r="M84" s="48" t="s">
         <v>441</v>
       </c>
@@ -16433,7 +17776,7 @@
       <c r="K85" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L85" s="84"/>
+      <c r="L85" s="98"/>
       <c r="M85" s="48" t="s">
         <v>448</v>
       </c>
@@ -16462,7 +17805,7 @@
       </c>
       <c r="J86" s="24"/>
       <c r="K86" s="24"/>
-      <c r="L86" s="84"/>
+      <c r="L86" s="98"/>
       <c r="M86" s="48" t="s">
         <v>449</v>
       </c>
@@ -16491,7 +17834,7 @@
       </c>
       <c r="J87" s="24"/>
       <c r="K87" s="24"/>
-      <c r="L87" s="84"/>
+      <c r="L87" s="98"/>
       <c r="M87" s="48" t="s">
         <v>450</v>
       </c>
@@ -16520,7 +17863,7 @@
       </c>
       <c r="J88" s="24"/>
       <c r="K88" s="24"/>
-      <c r="L88" s="84"/>
+      <c r="L88" s="98"/>
       <c r="M88" s="48" t="s">
         <v>450</v>
       </c>
@@ -16549,7 +17892,7 @@
       </c>
       <c r="J89" s="24"/>
       <c r="K89" s="24"/>
-      <c r="L89" s="84"/>
+      <c r="L89" s="98"/>
       <c r="M89" s="48" t="s">
         <v>451</v>
       </c>
@@ -16578,7 +17921,7 @@
       </c>
       <c r="J90" s="24"/>
       <c r="K90" s="24"/>
-      <c r="L90" s="84"/>
+      <c r="L90" s="98"/>
       <c r="M90" s="48" t="s">
         <v>451</v>
       </c>
@@ -16615,7 +17958,7 @@
       <c r="K91" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L91" s="84" t="s">
+      <c r="L91" s="98" t="s">
         <v>627</v>
       </c>
       <c r="M91" s="48"/>
@@ -16650,7 +17993,7 @@
       </c>
       <c r="J92" s="41"/>
       <c r="K92" s="41"/>
-      <c r="L92" s="84"/>
+      <c r="L92" s="98"/>
       <c r="M92" s="48"/>
     </row>
     <row r="93" spans="1:13">
@@ -16687,7 +18030,7 @@
       <c r="K93" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L93" s="84"/>
+      <c r="L93" s="98"/>
       <c r="M93" s="48"/>
     </row>
     <row r="94" spans="1:13">
@@ -16724,7 +18067,7 @@
       <c r="K94" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L94" s="84"/>
+      <c r="L94" s="98"/>
       <c r="M94" s="48"/>
     </row>
     <row r="95" spans="1:13">
@@ -16761,7 +18104,7 @@
       <c r="K95" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L95" s="84"/>
+      <c r="L95" s="98"/>
       <c r="M95" s="48"/>
     </row>
     <row r="96" spans="1:13">
@@ -16798,7 +18141,7 @@
       <c r="K96" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L96" s="84"/>
+      <c r="L96" s="98"/>
       <c r="M96" s="48"/>
     </row>
     <row r="97" spans="1:13">
@@ -16835,7 +18178,7 @@
       <c r="K97" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L97" s="84"/>
+      <c r="L97" s="98"/>
       <c r="M97" s="48"/>
     </row>
     <row r="98" spans="1:13">
@@ -16872,7 +18215,7 @@
       <c r="K98" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L98" s="84"/>
+      <c r="L98" s="98"/>
       <c r="M98" s="52" t="s">
         <v>452</v>
       </c>
@@ -16911,7 +18254,7 @@
       <c r="K99" s="41" t="s">
         <v>585</v>
       </c>
-      <c r="L99" s="84"/>
+      <c r="L99" s="98"/>
       <c r="M99" s="52" t="s">
         <v>452</v>
       </c>
@@ -16948,7 +18291,7 @@
       <c r="K100" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L100" s="84"/>
+      <c r="L100" s="98"/>
       <c r="M100" s="48" t="s">
         <v>453</v>
       </c>
@@ -16985,7 +18328,7 @@
       <c r="K101" s="41" t="s">
         <v>597</v>
       </c>
-      <c r="L101" s="84"/>
+      <c r="L101" s="98"/>
       <c r="M101" s="48" t="s">
         <v>453</v>
       </c>
@@ -17020,7 +18363,7 @@
       <c r="K102" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L102" s="84"/>
+      <c r="L102" s="98"/>
       <c r="M102" s="48" t="s">
         <v>454</v>
       </c>
@@ -17059,7 +18402,7 @@
       <c r="K103" s="41" t="s">
         <v>590</v>
       </c>
-      <c r="L103" s="84"/>
+      <c r="L103" s="98"/>
       <c r="M103" s="52" t="s">
         <v>452</v>
       </c>
@@ -17098,7 +18441,7 @@
       <c r="K104" s="24" t="s">
         <v>590</v>
       </c>
-      <c r="L104" s="84"/>
+      <c r="L104" s="98"/>
       <c r="M104" s="48" t="s">
         <v>455</v>
       </c>
@@ -19994,15 +21337,6 @@
     </row>
     <row r="202" spans="1:13">
       <c r="F202" s="58"/>
-    </row>
-    <row r="203" spans="1:13">
-      <c r="F203" s="58"/>
-    </row>
-    <row r="204" spans="1:13">
-      <c r="F204" s="58"/>
-    </row>
-    <row r="205" spans="1:13">
-      <c r="F205" s="58"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M183" xr:uid="{DB2252FB-561C-4694-B5F3-846A13872E41}"/>
@@ -20016,57 +21350,604 @@
     <mergeCell ref="L35:L76"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F2:F166 F168:F184 F206:F219">
-    <cfRule type="duplicateValues" dxfId="17" priority="23"/>
+  <conditionalFormatting sqref="F2:F166 F168:F184">
+    <cfRule type="duplicateValues" dxfId="18" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F202">
+    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F167">
-    <cfRule type="duplicateValues" dxfId="16" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F190">
-    <cfRule type="duplicateValues" dxfId="15" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F191">
-    <cfRule type="duplicateValues" dxfId="14" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F192">
-    <cfRule type="duplicateValues" dxfId="13" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F199">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F201">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G184">
-    <cfRule type="duplicateValues" dxfId="8" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G219">
-    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:G190">
-    <cfRule type="duplicateValues" dxfId="6" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G185:G219">
-    <cfRule type="duplicateValues" dxfId="5" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G191:G196">
-    <cfRule type="duplicateValues" dxfId="4" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G197:G198">
-    <cfRule type="duplicateValues" dxfId="3" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G199:G201">
-    <cfRule type="duplicateValues" dxfId="2" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G202:G211">
-    <cfRule type="duplicateValues" dxfId="1" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G212:G219">
-    <cfRule type="duplicateValues" dxfId="0" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8249AD-D1C2-4712-B9FE-673A7F5CBADC}">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="34.125" customWidth="1"/>
+    <col min="8" max="8" width="58.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="95" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" s="95" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="95" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" s="95" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="F1" s="95" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" s="95" t="s">
+        <v>214</v>
+      </c>
+      <c r="H1" s="95" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="17.25" thickBot="1">
+      <c r="A2" s="96"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>793</v>
+      </c>
+      <c r="B3">
+        <v>102</v>
+      </c>
+      <c r="C3">
+        <v>904</v>
+      </c>
+      <c r="D3" t="s">
+        <v>794</v>
+      </c>
+      <c r="F3" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>795</v>
+      </c>
+      <c r="B4">
+        <v>104</v>
+      </c>
+      <c r="C4">
+        <v>2002</v>
+      </c>
+      <c r="D4" t="s">
+        <v>796</v>
+      </c>
+      <c r="F4" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B5">
+        <v>105</v>
+      </c>
+      <c r="C5">
+        <v>1706</v>
+      </c>
+      <c r="D5" t="s">
+        <v>798</v>
+      </c>
+      <c r="F5" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>799</v>
+      </c>
+      <c r="B6">
+        <v>508</v>
+      </c>
+      <c r="C6">
+        <v>1903</v>
+      </c>
+      <c r="D6" t="s">
+        <v>800</v>
+      </c>
+      <c r="F6" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>799</v>
+      </c>
+      <c r="B7">
+        <v>506</v>
+      </c>
+      <c r="C7">
+        <v>1911</v>
+      </c>
+      <c r="D7" t="s">
+        <v>801</v>
+      </c>
+      <c r="F7" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>799</v>
+      </c>
+      <c r="B8">
+        <v>506</v>
+      </c>
+      <c r="C8">
+        <v>1912</v>
+      </c>
+      <c r="D8" t="s">
+        <v>802</v>
+      </c>
+      <c r="F8" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>799</v>
+      </c>
+      <c r="B9">
+        <v>506</v>
+      </c>
+      <c r="C9">
+        <v>1913</v>
+      </c>
+      <c r="D9" t="s">
+        <v>803</v>
+      </c>
+      <c r="F9" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>804</v>
+      </c>
+      <c r="B10">
+        <v>713</v>
+      </c>
+      <c r="C10">
+        <v>1501</v>
+      </c>
+      <c r="D10" t="s">
+        <v>805</v>
+      </c>
+      <c r="F10" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>804</v>
+      </c>
+      <c r="B11">
+        <v>716</v>
+      </c>
+      <c r="C11">
+        <v>1501</v>
+      </c>
+      <c r="D11" t="s">
+        <v>806</v>
+      </c>
+      <c r="F11" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>804</v>
+      </c>
+      <c r="B12">
+        <v>717</v>
+      </c>
+      <c r="C12">
+        <v>1501</v>
+      </c>
+      <c r="D12" t="s">
+        <v>807</v>
+      </c>
+      <c r="F12" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>804</v>
+      </c>
+      <c r="B13">
+        <v>718</v>
+      </c>
+      <c r="C13">
+        <v>1304</v>
+      </c>
+      <c r="D13" t="s">
+        <v>808</v>
+      </c>
+      <c r="F13" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>804</v>
+      </c>
+      <c r="B14">
+        <v>706</v>
+      </c>
+      <c r="C14">
+        <v>1501</v>
+      </c>
+      <c r="D14" t="s">
+        <v>809</v>
+      </c>
+      <c r="F14" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>810</v>
+      </c>
+      <c r="B15">
+        <v>205</v>
+      </c>
+      <c r="C15">
+        <v>1506</v>
+      </c>
+      <c r="D15" t="s">
+        <v>811</v>
+      </c>
+      <c r="F15" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>810</v>
+      </c>
+      <c r="B16">
+        <v>212</v>
+      </c>
+      <c r="C16">
+        <v>1504</v>
+      </c>
+      <c r="D16" t="s">
+        <v>812</v>
+      </c>
+      <c r="F16" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>813</v>
+      </c>
+      <c r="B17">
+        <v>106</v>
+      </c>
+      <c r="C17">
+        <v>204</v>
+      </c>
+      <c r="D17" t="s">
+        <v>814</v>
+      </c>
+      <c r="F17" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>815</v>
+      </c>
+      <c r="B18">
+        <v>2124</v>
+      </c>
+      <c r="C18">
+        <v>1001</v>
+      </c>
+      <c r="D18" t="s">
+        <v>816</v>
+      </c>
+      <c r="F18" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>817</v>
+      </c>
+      <c r="B19">
+        <v>101</v>
+      </c>
+      <c r="C19">
+        <v>1907</v>
+      </c>
+      <c r="D19" t="s">
+        <v>818</v>
+      </c>
+      <c r="F19" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>817</v>
+      </c>
+      <c r="B20">
+        <v>101</v>
+      </c>
+      <c r="C20">
+        <v>2007</v>
+      </c>
+      <c r="D20" t="s">
+        <v>819</v>
+      </c>
+      <c r="F20" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>817</v>
+      </c>
+      <c r="B21">
+        <v>101</v>
+      </c>
+      <c r="C21">
+        <v>1807</v>
+      </c>
+      <c r="D21" t="s">
+        <v>820</v>
+      </c>
+      <c r="F21" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>821</v>
+      </c>
+      <c r="B22">
+        <v>408</v>
+      </c>
+      <c r="C22">
+        <v>801</v>
+      </c>
+      <c r="D22" t="s">
+        <v>822</v>
+      </c>
+      <c r="F22" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>823</v>
+      </c>
+      <c r="B23">
+        <v>904</v>
+      </c>
+      <c r="C23">
+        <v>1504</v>
+      </c>
+      <c r="D23" t="s">
+        <v>824</v>
+      </c>
+      <c r="F23" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>823</v>
+      </c>
+      <c r="B24">
+        <v>905</v>
+      </c>
+      <c r="C24">
+        <v>1404</v>
+      </c>
+      <c r="D24" t="s">
+        <v>825</v>
+      </c>
+      <c r="F24" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>823</v>
+      </c>
+      <c r="B25">
+        <v>904</v>
+      </c>
+      <c r="C25">
+        <v>1404</v>
+      </c>
+      <c r="D25" t="s">
+        <v>826</v>
+      </c>
+      <c r="F25" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>823</v>
+      </c>
+      <c r="B26">
+        <v>908</v>
+      </c>
+      <c r="C26">
+        <v>1504</v>
+      </c>
+      <c r="D26" t="s">
+        <v>827</v>
+      </c>
+      <c r="F26" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>828</v>
+      </c>
+      <c r="B27">
+        <v>107</v>
+      </c>
+      <c r="C27">
+        <v>1301</v>
+      </c>
+      <c r="D27" t="s">
+        <v>829</v>
+      </c>
+      <c r="F27" s="92">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="100" t="s">
+        <v>544</v>
+      </c>
+      <c r="B28">
+        <v>102</v>
+      </c>
+      <c r="C28">
+        <v>1003</v>
+      </c>
+      <c r="D28" t="s">
+        <v>548</v>
+      </c>
+      <c r="F28" s="92">
+        <v>45191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>835</v>
+      </c>
+      <c r="B29">
+        <v>104</v>
+      </c>
+      <c r="C29">
+        <v>304</v>
+      </c>
+      <c r="D29" t="s">
+        <v>836</v>
+      </c>
+      <c r="F29" s="92">
+        <v>45191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>531</v>
+      </c>
+      <c r="B30">
+        <v>104</v>
+      </c>
+      <c r="C30">
+        <v>803</v>
+      </c>
+      <c r="D30" t="s">
+        <v>532</v>
+      </c>
+      <c r="F30" s="92">
+        <v>45191</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>